<commit_message>
update add and edit product
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hoctap\SoftwareTesting\software_testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C90B9BEC-F067-4349-A18C-C7D52DCA570B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E4BDC01-A8FB-4E68-A004-431C1E3C8BB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Đăng nhập(khách hàng)" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Đăng nhập(admin)" sheetId="3" r:id="rId3"/>
     <sheet name="Tìm Kiếm" sheetId="4" r:id="rId4"/>
     <sheet name="Thanh toán" sheetId="5" r:id="rId5"/>
+    <sheet name="Thêm sản phẩm" sheetId="6" r:id="rId6"/>
+    <sheet name="Sửa sản phẩm" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
   <si>
     <t>tester@123</t>
   </si>
@@ -131,6 +133,60 @@
   </si>
   <si>
     <t>9704198526191432198</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>brand</t>
+  </si>
+  <si>
+    <t>price</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Đồng hồ siêu cấp smartwatch</t>
+  </si>
+  <si>
+    <t>D:\admin.png</t>
+  </si>
+  <si>
+    <t>Đồng hồ</t>
+  </si>
+  <si>
+    <t>Casio</t>
+  </si>
+  <si>
+    <t>Điện tử</t>
+  </si>
+  <si>
+    <t>Đồng hồ siêu cấp smartwatch 2</t>
+  </si>
+  <si>
+    <t>Đồng hồ 2</t>
+  </si>
+  <si>
+    <t>Casio 2</t>
+  </si>
+  <si>
+    <t>Đồng hồ siêu cấp smartwatch 21212</t>
+  </si>
+  <si>
+    <t>Đồng hồ 2121</t>
+  </si>
+  <si>
+    <t>Đồng hồ siêu cấp smartwatch 2 212112</t>
+  </si>
+  <si>
+    <t>Điện tử 21</t>
   </si>
 </sst>
 </file>
@@ -781,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AA6E072-0489-4376-B02A-47EF7F863343}">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -857,4 +913,226 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C848A44-E0E4-4926-90B4-A29B166C8D79}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{872AC129-8B24-49BC-A794-CB2DC0F76CC2}">
+  <dimension ref="A1:H4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>